<commit_message>
fixed excel mistake with parameter kappaYieldH
</commit_message>
<xml_diff>
--- a/data/Chile-Madhura/input_data/hydro_cascades.xlsx
+++ b/data/Chile-Madhura/input_data/hydro_cascades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70b0e526faaa1b23/Dokumente/Alles zum Studium/Master/Masterarbeit/Leelo/data/TestLocation/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70b0e526faaa1b23/Dokumente/Alles zum Studium/Master/Masterarbeit/Leelo/data/Chile-Madhura/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39A60DF3-B148-4230-9ABF-49A3163EA0E0}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACD3D1C8-A27A-418F-A5AF-B7D1C3F8B903}"/>
   <bookViews>
-    <workbookView xWindow="4356" yWindow="2808" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13600" yWindow="-17090" windowWidth="12440" windowHeight="6320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -855,7 +855,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,8 +1097,8 @@
         <v>181.4</v>
       </c>
       <c r="L3" s="11">
-        <f>I3*J3*9.8/1000</f>
-        <v>9.7710900000000009</v>
+        <f>J3*K3*9.8/1000</f>
+        <v>1.5110620000000001</v>
       </c>
       <c r="M3" s="6">
         <v>1033.5</v>
@@ -1187,8 +1187,8 @@
         <v>125.8</v>
       </c>
       <c r="L4" s="11">
-        <f>I4*J4*9.8/1000</f>
-        <v>0.37367400000000006</v>
+        <f t="shared" ref="L4:L42" si="0">J4*K4*9.8/1000</f>
+        <v>1.1465412000000001</v>
       </c>
       <c r="M4" s="4">
         <v>32</v>
@@ -1277,8 +1277,8 @@
         <v>99</v>
       </c>
       <c r="L5" s="11">
-        <f t="shared" ref="L5:L42" si="0">I5*J5*9.8/1000</f>
-        <v>44.1</v>
+        <f t="shared" si="0"/>
+        <v>0.87318000000000018</v>
       </c>
       <c r="M5" s="4">
         <v>699</v>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="L6" s="11">
         <f t="shared" si="0"/>
-        <v>9.9224999999999994</v>
+        <v>0.44100000000000006</v>
       </c>
       <c r="M6" s="4">
         <v>492</v>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="L7" s="11">
         <f t="shared" si="0"/>
-        <v>48.632304000000012</v>
+        <v>4.8015590000000001</v>
       </c>
       <c r="M7" s="7">
         <v>673.11</v>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="L8" s="11">
         <f t="shared" si="0"/>
-        <v>2.204118E-4</v>
+        <v>1.2000198</v>
       </c>
       <c r="M8" s="4">
         <v>129</v>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="L9" s="11">
         <f t="shared" si="0"/>
-        <v>5.6977200000000007E-3</v>
+        <v>1.5827</v>
       </c>
       <c r="M9" s="7">
         <v>478.76</v>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="L10" s="11">
         <f t="shared" si="0"/>
-        <v>4.2791112000000013E-3</v>
+        <v>1.2800760000000002</v>
       </c>
       <c r="M10" s="7">
         <v>267.2</v>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="L11" s="11">
         <f t="shared" si="0"/>
-        <v>4.2653520000000009E-3</v>
+        <v>0.54091590000000012</v>
       </c>
       <c r="M11" s="7">
         <v>70.650000000000006</v>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="L13" s="11">
         <f t="shared" si="0"/>
-        <v>9.7064100000000018</v>
+        <v>1.9321680000000001</v>
       </c>
       <c r="M13" s="7">
         <v>257.36</v>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="L14" s="11">
         <f t="shared" si="0"/>
-        <v>4.7064500000000011</v>
+        <v>0.63308000000000009</v>
       </c>
       <c r="M14" s="7">
         <v>564.96</v>
@@ -2177,8 +2177,8 @@
         <v>370</v>
       </c>
       <c r="L15" s="11">
-        <f>I15*J15*9.8/1000</f>
-        <v>1.4112</v>
+        <f t="shared" si="0"/>
+        <v>2.9008000000000003</v>
       </c>
       <c r="M15" s="7">
         <v>105.82</v>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="L16" s="11">
         <f t="shared" si="0"/>
-        <v>11.978714538</v>
+        <v>5.9382168999999996</v>
       </c>
       <c r="M16" s="4">
         <v>150</v>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="L17" s="11">
         <f t="shared" si="0"/>
-        <v>2.6671680000000001E-3</v>
+        <v>0.8202600000000001</v>
       </c>
       <c r="M17" s="7">
         <v>69.88</v>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="L18" s="11">
         <f t="shared" si="0"/>
-        <v>2.6730950400000006E-3</v>
+        <v>1.0103662800000002</v>
       </c>
       <c r="M18" s="7">
         <v>91.77</v>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="L19" s="11">
         <f t="shared" si="0"/>
-        <v>2.6671680000000001E-3</v>
+        <v>0.44452800000000003</v>
       </c>
       <c r="M19" s="7">
         <v>39.93</v>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="L21" s="11">
         <f t="shared" si="0"/>
-        <v>1.11622</v>
+        <v>1.7159800000000001</v>
       </c>
       <c r="M21" s="7">
         <v>852.45</v>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="L22" s="11">
         <f t="shared" si="0"/>
-        <v>13.917960000000001</v>
+        <v>1.4817600000000002</v>
       </c>
       <c r="M22" s="7">
         <v>709.23</v>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="L23" s="11">
         <f t="shared" si="0"/>
-        <v>0.14660800000000004</v>
+        <v>0.31908800000000004</v>
       </c>
       <c r="M23" s="7">
         <v>94.76</v>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="L24" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.97020000000000006</v>
       </c>
       <c r="M24" s="7">
         <v>19.16</v>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="L25" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.18995340000000005</v>
       </c>
       <c r="M25" s="7">
         <v>36.909999999999997</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="L26" s="11">
         <f t="shared" si="0"/>
-        <v>7.1679999999999999E-3</v>
+        <v>1.5523200000000001</v>
       </c>
       <c r="M26" s="4">
         <v>112</v>
@@ -3258,7 +3258,7 @@
       </c>
       <c r="L27" s="11">
         <f t="shared" si="0"/>
-        <v>6.3262372881355946E-3</v>
+        <v>1.3194720000000002</v>
       </c>
       <c r="M27" s="4">
         <v>99.8</v>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="L28" s="11">
         <f t="shared" si="0"/>
-        <v>2.2049999999999999E-3</v>
+        <v>3.9249000000000001</v>
       </c>
       <c r="M28" s="4">
         <v>40</v>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="L29" s="11">
         <f t="shared" si="0"/>
-        <v>3.3516000000000002E-3</v>
+        <v>3.9249000000000001</v>
       </c>
       <c r="M29" s="4">
         <v>60</v>
@@ -3528,7 +3528,7 @@
       </c>
       <c r="L30" s="11">
         <f t="shared" si="0"/>
-        <v>9.8960400000000018E-3</v>
+        <v>3.1820599999999999</v>
       </c>
       <c r="M30" s="4">
         <v>237</v>
@@ -3618,7 +3618,7 @@
       </c>
       <c r="L31" s="11">
         <f t="shared" si="0"/>
-        <v>2.7588959999999998E-3</v>
+        <v>3.1015040000000003</v>
       </c>
       <c r="M31" s="4">
         <v>232.5</v>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="L32" s="11">
         <f t="shared" si="0"/>
-        <v>3.0710534400000011E-3</v>
+        <v>2.1509040000000006</v>
       </c>
       <c r="M32" s="4">
         <v>77</v>
@@ -3798,7 +3798,7 @@
       </c>
       <c r="L33" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0693760000000001</v>
       </c>
       <c r="M33" s="4">
         <v>49</v>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="L34" s="11">
         <f t="shared" si="0"/>
-        <v>1.5833664000000005E-3</v>
+        <v>4.5815000000000001</v>
       </c>
       <c r="M34" s="4">
         <v>55</v>
@@ -3978,7 +3978,7 @@
       </c>
       <c r="L35" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.6787160000000005</v>
       </c>
       <c r="M35" s="4">
         <v>94</v>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="L36" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.7796800000000004</v>
       </c>
       <c r="M36" s="4">
         <v>39</v>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="L37" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1907000000000001</v>
       </c>
       <c r="M37" s="4">
         <v>25</v>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="L38" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.9976000000000003</v>
       </c>
       <c r="M38" s="4">
         <v>267</v>
@@ -4338,7 +4338,7 @@
       </c>
       <c r="L39" s="11">
         <f t="shared" si="0"/>
-        <v>8.8199999999999997E-4</v>
+        <v>1.323</v>
       </c>
       <c r="M39" s="4">
         <v>30</v>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="L40" s="11">
         <f t="shared" si="0"/>
-        <v>3.8102400000000002E-2</v>
+        <v>0.42336000000000007</v>
       </c>
       <c r="M40" s="4">
         <v>51</v>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="L41" s="11">
         <f t="shared" si="0"/>
-        <v>1.8708199999999999</v>
+        <v>0.26028800000000002</v>
       </c>
       <c r="M41" s="4">
         <v>39</v>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="L42" s="11">
         <f t="shared" si="0"/>
-        <v>1.4126700000000002E-2</v>
+        <v>0.31443300000000007</v>
       </c>
       <c r="M42" s="4">
         <v>55</v>

</xml_diff>